<commit_message>
added categories to ag dataset
</commit_message>
<xml_diff>
--- a/Working files/Lists.xlsx
+++ b/Working files/Lists.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CJHx6\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfccdeabb580c92e/AI_Class/GIT/Project1/Working files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566FAC68-BFB2-4662-AD21-EE3B820EBC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{566FAC68-BFB2-4662-AD21-EE3B820EBC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEFEE9E6-3F4E-4D0D-A750-6DF86F39276B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{9038F32F-E838-4B1D-8754-D00D78CD3F50}"/>
   </bookViews>
@@ -690,12 +690,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -710,10 +716,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1050,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31ACCFA7-A5C5-49B9-8990-DD70674B34B8}">
   <dimension ref="A1:B197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1796,50 +1803,50 @@
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+      <c r="A93" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+      <c r="A94" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+      <c r="A95" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+      <c r="A96" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+      <c r="A97" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+      <c r="A98" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="3" t="s">
         <v>199</v>
       </c>
     </row>
@@ -1908,18 +1915,18 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+      <c r="A107" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+      <c r="A108" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="3" t="s">
         <v>199</v>
       </c>
     </row>
@@ -1932,10 +1939,10 @@
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+      <c r="A110" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="3" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2052,26 +2059,26 @@
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
+      <c r="A125" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
+      <c r="A126" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
+      <c r="A127" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="3" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2084,26 +2091,26 @@
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+      <c r="A129" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+      <c r="A130" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
+      <c r="A131" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="3" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2116,26 +2123,26 @@
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+      <c r="A133" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+      <c r="A134" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+      <c r="A135" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="3" t="s">
         <v>199</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified List_test.csv, and updated code for more specific graphs
</commit_message>
<xml_diff>
--- a/Working files/Lists.xlsx
+++ b/Working files/Lists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfccdeabb580c92e/AI_Class/GIT/Project1/Working files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{566FAC68-BFB2-4662-AD21-EE3B820EBC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEFEE9E6-3F4E-4D0D-A750-6DF86F39276B}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{566FAC68-BFB2-4662-AD21-EE3B820EBC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{597DBA0F-83E3-4FE5-BF1C-27ACA1AF0934}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{9038F32F-E838-4B1D-8754-D00D78CD3F50}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="208">
   <si>
     <t>Item</t>
   </si>
@@ -736,6 +736,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1055,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31ACCFA7-A5C5-49B9-8990-DD70674B34B8}">
-  <dimension ref="A1:B197"/>
+  <dimension ref="A1:B195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96:XFD96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1828,7 +1832,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>199</v>
@@ -1836,23 +1840,23 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B98" s="3" t="s">
+      <c r="A98" t="s">
+        <v>93</v>
+      </c>
+      <c r="B98" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="B99" t="s">
         <v>199</v>
@@ -1860,7 +1864,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B100" t="s">
         <v>199</v>
@@ -1868,7 +1872,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="B101" t="s">
         <v>199</v>
@@ -1876,7 +1880,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>94</v>
+        <v>17</v>
       </c>
       <c r="B102" t="s">
         <v>199</v>
@@ -1884,7 +1888,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B103" t="s">
         <v>199</v>
@@ -1892,7 +1896,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="B104" t="s">
         <v>199</v>
@@ -1900,55 +1904,55 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="B105" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
-        <v>20</v>
-      </c>
-      <c r="B106" t="s">
+      <c r="A106" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B106" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B108" s="3" t="s">
+      <c r="A108" t="s">
+        <v>100</v>
+      </c>
+      <c r="B108" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
-        <v>100</v>
-      </c>
-      <c r="B109" t="s">
+      <c r="A109" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B109" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B110" s="3" t="s">
+      <c r="A110" t="s">
+        <v>157</v>
+      </c>
+      <c r="B110" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>157</v>
+        <v>104</v>
       </c>
       <c r="B111" t="s">
         <v>199</v>
@@ -1956,7 +1960,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>104</v>
+        <v>26</v>
       </c>
       <c r="B112" t="s">
         <v>199</v>
@@ -1964,7 +1968,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B113" t="s">
         <v>199</v>
@@ -1972,7 +1976,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B114" t="s">
         <v>199</v>
@@ -1980,7 +1984,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="B115" t="s">
         <v>199</v>
@@ -1988,7 +1992,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B116" t="s">
         <v>199</v>
@@ -1996,7 +2000,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
       <c r="B117" t="s">
         <v>199</v>
@@ -2004,7 +2008,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>29</v>
+        <v>160</v>
       </c>
       <c r="B118" t="s">
         <v>199</v>
@@ -2012,7 +2016,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="B119" t="s">
         <v>199</v>
@@ -2020,7 +2024,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>105</v>
+        <v>192</v>
       </c>
       <c r="B120" t="s">
         <v>199</v>
@@ -2028,7 +2032,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>192</v>
+        <v>135</v>
       </c>
       <c r="B121" t="s">
         <v>199</v>
@@ -2036,7 +2040,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>135</v>
+        <v>30</v>
       </c>
       <c r="B122" t="s">
         <v>199</v>
@@ -2044,23 +2048,23 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="B123" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
-        <v>106</v>
-      </c>
-      <c r="B124" t="s">
+      <c r="A124" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B124" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>199</v>
@@ -2068,87 +2072,87 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B127" s="3" t="s">
+      <c r="A127" t="s">
+        <v>112</v>
+      </c>
+      <c r="B127" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
-        <v>112</v>
-      </c>
-      <c r="B128" t="s">
+      <c r="A128" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B128" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B130" s="3" t="s">
+      <c r="A130" t="s">
+        <v>74</v>
+      </c>
+      <c r="B130" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
-        <v>74</v>
-      </c>
-      <c r="B132" t="s">
+      <c r="A132" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B132" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
-        <v>75</v>
+        <v>126</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A134" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>199</v>
+      <c r="A134" t="s">
+        <v>1</v>
+      </c>
+      <c r="B134" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>199</v>
+      <c r="A135" t="s">
+        <v>183</v>
+      </c>
+      <c r="B135" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>1</v>
+        <v>191</v>
       </c>
       <c r="B136" t="s">
         <v>197</v>
@@ -2156,7 +2160,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>183</v>
+        <v>141</v>
       </c>
       <c r="B137" t="s">
         <v>197</v>
@@ -2164,7 +2168,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>191</v>
+        <v>88</v>
       </c>
       <c r="B138" t="s">
         <v>197</v>
@@ -2172,7 +2176,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B139" t="s">
         <v>197</v>
@@ -2180,7 +2184,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>88</v>
+        <v>167</v>
       </c>
       <c r="B140" t="s">
         <v>197</v>
@@ -2188,7 +2192,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>132</v>
+        <v>189</v>
       </c>
       <c r="B141" t="s">
         <v>197</v>
@@ -2196,7 +2200,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>167</v>
+        <v>190</v>
       </c>
       <c r="B142" t="s">
         <v>197</v>
@@ -2204,7 +2208,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>189</v>
+        <v>40</v>
       </c>
       <c r="B143" t="s">
         <v>197</v>
@@ -2212,7 +2216,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>190</v>
+        <v>45</v>
       </c>
       <c r="B144" t="s">
         <v>197</v>
@@ -2220,7 +2224,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="B145" t="s">
         <v>197</v>
@@ -2228,7 +2232,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>45</v>
+        <v>163</v>
       </c>
       <c r="B146" t="s">
         <v>197</v>
@@ -2236,7 +2240,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B147" t="s">
         <v>197</v>
@@ -2244,23 +2248,23 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="B148" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B149" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>185</v>
+        <v>57</v>
       </c>
       <c r="B150" t="s">
         <v>202</v>
@@ -2268,23 +2272,23 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="B151" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>57</v>
+        <v>152</v>
       </c>
       <c r="B152" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>127</v>
+        <v>193</v>
       </c>
       <c r="B153" t="s">
         <v>198</v>
@@ -2292,7 +2296,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="B154" t="s">
         <v>198</v>
@@ -2300,7 +2304,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>193</v>
+        <v>80</v>
       </c>
       <c r="B155" t="s">
         <v>198</v>
@@ -2308,7 +2312,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B156" t="s">
         <v>198</v>
@@ -2316,7 +2320,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B157" t="s">
         <v>198</v>
@@ -2324,7 +2328,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B158" t="s">
         <v>198</v>
@@ -2332,7 +2336,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>83</v>
+        <v>142</v>
       </c>
       <c r="B159" t="s">
         <v>198</v>
@@ -2340,7 +2344,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B160" t="s">
         <v>198</v>
@@ -2348,7 +2352,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B161" t="s">
         <v>198</v>
@@ -2356,7 +2360,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>85</v>
+        <v>187</v>
       </c>
       <c r="B162" t="s">
         <v>198</v>
@@ -2364,7 +2368,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B163" t="s">
         <v>198</v>
@@ -2372,7 +2376,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>187</v>
+        <v>89</v>
       </c>
       <c r="B164" t="s">
         <v>198</v>
@@ -2380,7 +2384,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>131</v>
+        <v>169</v>
       </c>
       <c r="B165" t="s">
         <v>198</v>
@@ -2388,7 +2392,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B166" t="s">
         <v>198</v>
@@ -2396,7 +2400,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="B167" t="s">
         <v>198</v>
@@ -2404,7 +2408,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B168" t="s">
         <v>198</v>
@@ -2412,7 +2416,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>188</v>
+        <v>156</v>
       </c>
       <c r="B169" t="s">
         <v>198</v>
@@ -2420,7 +2424,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="B170" t="s">
         <v>198</v>
@@ -2428,7 +2432,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>156</v>
+        <v>99</v>
       </c>
       <c r="B171" t="s">
         <v>198</v>
@@ -2436,7 +2440,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>171</v>
+        <v>101</v>
       </c>
       <c r="B172" t="s">
         <v>198</v>
@@ -2444,7 +2448,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="B173" t="s">
         <v>198</v>
@@ -2452,7 +2456,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B174" t="s">
         <v>198</v>
@@ -2460,7 +2464,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B175" t="s">
         <v>198</v>
@@ -2468,7 +2472,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B176" t="s">
         <v>198</v>
@@ -2476,7 +2480,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="B177" t="s">
         <v>198</v>
@@ -2484,7 +2488,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>107</v>
+        <v>35</v>
       </c>
       <c r="B178" t="s">
         <v>198</v>
@@ -2492,7 +2496,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B179" t="s">
         <v>198</v>
@@ -2500,7 +2504,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="B180" t="s">
         <v>198</v>
@@ -2508,7 +2512,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>110</v>
+        <v>42</v>
       </c>
       <c r="B181" t="s">
         <v>198</v>
@@ -2516,7 +2520,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="B182" t="s">
         <v>198</v>
@@ -2524,7 +2528,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="B183" t="s">
         <v>198</v>
@@ -2532,7 +2536,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>137</v>
+        <v>181</v>
       </c>
       <c r="B184" t="s">
         <v>198</v>
@@ -2540,7 +2544,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="B185" t="s">
         <v>198</v>
@@ -2548,7 +2552,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>181</v>
+        <v>114</v>
       </c>
       <c r="B186" t="s">
         <v>198</v>
@@ -2556,7 +2560,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B187" t="s">
         <v>198</v>
@@ -2564,7 +2568,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B188" t="s">
         <v>198</v>
@@ -2572,7 +2576,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="B189" t="s">
         <v>198</v>
@@ -2580,7 +2584,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>121</v>
+        <v>56</v>
       </c>
       <c r="B190" t="s">
         <v>198</v>
@@ -2588,7 +2592,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="B191" t="s">
         <v>198</v>
@@ -2596,7 +2600,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>56</v>
+        <v>149</v>
       </c>
       <c r="B192" t="s">
         <v>198</v>
@@ -2604,7 +2608,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B193" t="s">
         <v>198</v>
@@ -2612,7 +2616,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="B194" t="s">
         <v>198</v>
@@ -2620,31 +2624,15 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="B195" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A196" t="s">
-        <v>78</v>
-      </c>
-      <c r="B196" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A197" t="s">
-        <v>150</v>
-      </c>
-      <c r="B197" t="s">
-        <v>198</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B254">
-    <sortCondition ref="B2:B254"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B252">
+    <sortCondition ref="B2:B252"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>